<commit_message>
Updated table images (v5)
</commit_message>
<xml_diff>
--- a/docs/Metrics for Hypothetical Plans.xlsx
+++ b/docs/Metrics for Hypothetical Plans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11205"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/dev/bias-irl/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/dev/bias-irl/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03DFCA6-CB68-D147-8551-EB0665C8095D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE22E189-438C-CA4A-9F4D-5F8E6F6FCA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="500" windowWidth="27540" windowHeight="17500" activeTab="1" xr2:uid="{F08C87BC-C96D-1A4F-8DA4-EEEA4D15A1AA}"/>
+    <workbookView xWindow="1400" yWindow="520" windowWidth="27540" windowHeight="17500" activeTab="1" xr2:uid="{F08C87BC-C96D-1A4F-8DA4-EEEA4D15A1AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 5-1a" sheetId="5" r:id="rId1"/>
@@ -621,13 +621,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -644,38 +643,29 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -692,8 +682,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -708,9 +697,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -731,7 +717,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -742,16 +728,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -766,17 +743,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -791,9 +761,6 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -833,42 +800,82 @@
     <xf numFmtId="164" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1209,1414 +1216,1404 @@
     <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.83203125" style="2" customWidth="1"/>
     <col min="10" max="10" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.83203125" style="5" customWidth="1"/>
-    <col min="21" max="21" width="10.83203125" style="18"/>
+    <col min="18" max="18" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="49" t="s">
+      <c r="B1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="M1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="48" t="s">
+      <c r="N1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="49" t="s">
+      <c r="O1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="49" t="s">
+      <c r="P1" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="Q1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="49" t="s">
+      <c r="R1" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="52" t="s">
+      <c r="S1" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="10"/>
-      <c r="U1" s="6" t="s">
+      <c r="T1" s="9"/>
+      <c r="U1" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="59">
+      <c r="B2" s="49">
         <v>0.6</v>
       </c>
-      <c r="C2" s="60">
+      <c r="C2" s="50">
         <v>0.60029999999999994</v>
       </c>
-      <c r="D2" s="61">
+      <c r="D2" s="51">
         <v>1.0033000000000001</v>
       </c>
-      <c r="E2" s="62">
+      <c r="E2" s="52">
         <v>0.84309999999999996</v>
       </c>
-      <c r="F2" s="62">
+      <c r="F2" s="52">
         <v>0.98609999999999998</v>
       </c>
-      <c r="G2" s="61">
+      <c r="G2" s="51">
         <v>4.9264000000000001</v>
       </c>
-      <c r="H2" s="60">
+      <c r="H2" s="50">
         <v>0.1171</v>
       </c>
-      <c r="I2" s="60">
-        <v>0</v>
-      </c>
-      <c r="J2" s="59">
-        <v>0</v>
-      </c>
-      <c r="K2" s="60">
-        <v>0</v>
-      </c>
-      <c r="L2" s="60">
+      <c r="I2" s="50">
+        <v>0</v>
+      </c>
+      <c r="J2" s="49">
+        <v>0</v>
+      </c>
+      <c r="K2" s="50">
+        <v>0</v>
+      </c>
+      <c r="L2" s="50">
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="M2" s="60">
+      <c r="M2" s="50">
         <v>-3.6299999999999999E-2</v>
       </c>
-      <c r="N2" s="59">
+      <c r="N2" s="49">
         <v>-2.9999999999999997E-4</v>
       </c>
-      <c r="O2" s="60">
+      <c r="O2" s="50">
         <v>9.9699999999999997E-2</v>
       </c>
-      <c r="P2" s="60">
+      <c r="P2" s="50">
         <v>-1.6E-2</v>
       </c>
-      <c r="Q2" s="59">
+      <c r="Q2" s="49">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="R2" s="60">
+      <c r="R2" s="50">
         <v>-6.7999999999999996E-3</v>
       </c>
-      <c r="S2" s="63">
+      <c r="S2" s="53">
         <v>-0.15540000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="43" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="4">
         <v>0.6</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="2">
         <v>0.69199999999999995</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>1.92</v>
       </c>
-      <c r="E3" s="40">
+      <c r="E3" s="3">
         <v>1.6133999999999999</v>
       </c>
-      <c r="F3" s="40">
+      <c r="F3" s="3">
         <v>0.41980000000000001</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <v>1.2159</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="2">
         <v>0.1028</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="2">
         <v>0</v>
       </c>
       <c r="J3" s="4">
         <v>0</v>
       </c>
-      <c r="K3" s="5">
-        <v>0</v>
-      </c>
-      <c r="L3" s="5">
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
         <v>4.7300000000000002E-2</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="2">
         <v>-2.64E-2</v>
       </c>
       <c r="N3" s="4">
         <v>-9.1999999999999998E-2</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="2">
         <v>-3.0700000000000002E-2</v>
       </c>
       <c r="Q3" s="4">
         <v>-9.1999999999999998E-2</v>
       </c>
-      <c r="R3" s="5">
+      <c r="R3" s="2">
         <v>-9.9900000000000003E-2</v>
       </c>
-      <c r="S3" s="54">
+      <c r="S3" s="44">
         <v>-2.4965000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="43" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="4">
         <v>0.6</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="2">
         <v>0.79769999999999996</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>2.9767000000000001</v>
       </c>
-      <c r="E4" s="40">
+      <c r="E4" s="3">
         <v>2.4315000000000002</v>
       </c>
-      <c r="F4" s="40">
+      <c r="F4" s="3">
         <v>0.21129999999999999</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <v>5.944</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="2">
         <v>0.109</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="2">
         <v>0</v>
       </c>
       <c r="J4" s="4">
         <v>0</v>
       </c>
-      <c r="K4" s="5">
-        <v>0</v>
-      </c>
-      <c r="L4" s="5">
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
         <v>5.1499999999999997E-2</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="2">
         <v>-1.7299999999999999E-2</v>
       </c>
       <c r="N4" s="4">
         <v>-0.19769999999999999</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="2">
         <v>-9.7699999999999995E-2</v>
       </c>
-      <c r="P4" s="5">
+      <c r="P4" s="2">
         <v>-5.45E-2</v>
       </c>
       <c r="Q4" s="4">
         <v>-0.19769999999999999</v>
       </c>
-      <c r="R4" s="5">
+      <c r="R4" s="2">
         <v>-0.2041</v>
       </c>
-      <c r="S4" s="54">
+      <c r="S4" s="44">
         <v>-5.1029999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="43" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="4">
         <v>0.64</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="2">
         <v>0.98380000000000001</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>3.456</v>
       </c>
-      <c r="E5" s="40">
+      <c r="E5" s="3">
         <v>0.74709999999999999</v>
       </c>
-      <c r="F5" s="40">
+      <c r="F5" s="3">
         <v>1.1385000000000001</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="55" t="s">
+      <c r="H5" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="2">
         <v>0</v>
       </c>
       <c r="J5" s="4">
         <v>0</v>
       </c>
-      <c r="K5" s="5">
-        <v>0</v>
-      </c>
-      <c r="L5" s="5">
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="2">
         <v>-8.0000000000000002E-3</v>
       </c>
       <c r="N5" s="4">
         <v>-0.34379999999999999</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="2">
         <v>-0.20380000000000001</v>
       </c>
-      <c r="P5" s="5">
+      <c r="P5" s="2">
         <v>-0.37919999999999998</v>
       </c>
       <c r="Q5" s="4">
         <v>-0.38379999999999997</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5" s="2">
         <v>-0.35410000000000003</v>
       </c>
-      <c r="S5" s="54">
+      <c r="S5" s="44">
         <v>-3.5405000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="43" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="4">
         <v>0.52</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="2">
         <v>0.66649999999999998</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <v>8.3239000000000001</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="3">
         <v>8.0289000000000001</v>
       </c>
-      <c r="F6" s="40">
+      <c r="F6" s="3">
         <v>2.46E-2</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="2">
         <v>2.58E-2</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="2">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="J6" s="4">
         <v>1.5E-3</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="2">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="2">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="2">
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="N6" s="4">
         <v>-0.14649999999999999</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="2">
         <v>-0.1265</v>
       </c>
-      <c r="P6" s="5">
+      <c r="P6" s="2">
         <v>-5.8999999999999999E-3</v>
       </c>
       <c r="Q6" s="4">
         <v>-0.16650000000000001</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R6" s="2">
         <v>-0.13150000000000001</v>
       </c>
-      <c r="S6" s="54">
+      <c r="S6" s="44">
         <v>-1.5783</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="43" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="4">
         <v>0.51</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="2">
         <v>0.56569999999999998</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>6.5736999999999997</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="3">
         <v>4.9969999999999999</v>
       </c>
-      <c r="F7" s="40">
+      <c r="F7" s="3">
         <v>0.10009999999999999</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <v>-0.7359</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="2">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="2">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="J7" s="4">
         <v>-1.49E-2</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="2">
         <v>-2.8E-3</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="2">
         <v>-1.34E-2</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="2">
         <v>-3.5999999999999999E-3</v>
       </c>
       <c r="N7" s="4">
         <v>-5.57E-2</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="2">
         <v>-4.5699999999999998E-2</v>
       </c>
-      <c r="P7" s="5">
+      <c r="P7" s="2">
         <v>-1.5800000000000002E-2</v>
       </c>
       <c r="Q7" s="4">
         <v>-6.5699999999999995E-2</v>
       </c>
-      <c r="R7" s="5">
+      <c r="R7" s="2">
         <v>-0.05</v>
       </c>
-      <c r="S7" s="54">
+      <c r="S7" s="44">
         <v>-0.4995</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="43" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="4">
         <v>0.52300000000000002</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="2">
         <v>0.59930000000000005</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>4.3182999999999998</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="3">
         <v>5.4100000000000002E-2</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="3">
         <v>18.401199999999999</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="11">
         <v>-15.289400000000001</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="2">
         <v>-2.9399999999999999E-2</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="2">
         <v>-9.1999999999999998E-2</v>
       </c>
       <c r="J8" s="4">
         <v>-9.6100000000000005E-2</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="2">
         <v>-6.7000000000000004E-2</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="2">
         <v>-9.1800000000000007E-2</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="2">
         <v>-4.6100000000000002E-2</v>
       </c>
       <c r="N8" s="4">
         <v>-7.6300000000000007E-2</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="2">
         <v>-5.33E-2</v>
       </c>
-      <c r="P8" s="5">
+      <c r="P8" s="2">
         <v>-9.8100000000000007E-2</v>
       </c>
       <c r="Q8" s="4">
         <v>-9.9299999999999999E-2</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="2">
         <v>-9.8500000000000004E-2</v>
       </c>
-      <c r="S8" s="54">
+      <c r="S8" s="44">
         <v>-0.98529999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="43" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="4">
         <v>0.52300000000000002</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="2">
         <v>0.6</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <v>4.3478000000000003</v>
       </c>
-      <c r="E9" s="40">
-        <v>0</v>
-      </c>
-      <c r="F9" s="66" t="s">
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="11">
         <v>-18.093499999999999</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="2">
         <v>-0.08</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="2">
         <v>-0.192</v>
       </c>
       <c r="J9" s="4">
         <v>-0.1</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="2">
         <v>-0.12609999999999999</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="2">
         <v>-0.1</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="2">
         <v>-7.9699999999999993E-2</v>
       </c>
       <c r="N9" s="4">
         <v>-7.6999999999999999E-2</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O9" s="2">
         <v>-5.3999999999999999E-2</v>
       </c>
-      <c r="P9" s="5">
+      <c r="P9" s="2">
         <v>-0.1</v>
       </c>
       <c r="Q9" s="4">
         <v>-0.1</v>
       </c>
-      <c r="R9" s="5">
+      <c r="R9" s="2">
         <v>-0.1</v>
       </c>
-      <c r="S9" s="54">
+      <c r="S9" s="44">
         <v>-1</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="43" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="4">
         <v>0.56999999999999995</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="2">
         <v>0.73980000000000001</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="11">
         <v>3.4262000000000001</v>
       </c>
-      <c r="E10" s="40">
+      <c r="E10" s="3">
         <v>1.9415</v>
       </c>
-      <c r="F10" s="40">
+      <c r="F10" s="3">
         <v>0.31509999999999999</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="11">
         <v>-29.989699999999999</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="2">
         <v>-1.6E-2</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="2">
         <v>0</v>
       </c>
       <c r="J10" s="4">
         <v>0</v>
       </c>
-      <c r="K10" s="5">
-        <v>0</v>
-      </c>
-      <c r="L10" s="5">
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="2">
         <v>-1.3899999999999999E-2</v>
       </c>
       <c r="N10" s="4">
         <v>-0.16980000000000001</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="2">
         <v>-9.98E-2</v>
       </c>
-      <c r="P10" s="5">
+      <c r="P10" s="2">
         <v>-0.10390000000000001</v>
       </c>
       <c r="Q10" s="4">
         <v>-0.13980000000000001</v>
       </c>
-      <c r="R10" s="5">
+      <c r="R10" s="2">
         <v>-0.15509999999999999</v>
       </c>
-      <c r="S10" s="54">
+      <c r="S10" s="44">
         <v>-1.5513999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="43" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="4">
         <v>0.443</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="2">
         <v>0.55600000000000005</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <v>-0.98219999999999996</v>
       </c>
-      <c r="E11" s="40">
+      <c r="E11" s="3">
         <v>1.6238999999999999</v>
       </c>
-      <c r="F11" s="40">
+      <c r="F11" s="3">
         <v>0.4158</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="11">
         <v>-29.011500000000002</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="2">
         <v>-0.15359999999999999</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="2">
         <v>-9.1999999999999998E-2</v>
       </c>
       <c r="J11" s="4">
         <v>-9.4899999999999998E-2</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="2">
         <v>-0.08</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="2">
         <v>-7.8299999999999995E-2</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="2">
         <v>-3.3599999999999998E-2</v>
       </c>
       <c r="N11" s="4">
         <v>-0.113</v>
       </c>
-      <c r="O11" s="5">
+      <c r="O11" s="2">
         <v>-0.17</v>
       </c>
-      <c r="P11" s="5">
+      <c r="P11" s="2">
         <v>-0.14849999999999999</v>
       </c>
       <c r="Q11" s="4">
         <v>-0.156</v>
       </c>
-      <c r="R11" s="5">
+      <c r="R11" s="2">
         <v>-0.1118</v>
       </c>
-      <c r="S11" s="54">
+      <c r="S11" s="44">
         <v>-1.1185</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="43" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="4">
         <v>0.5</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="2">
         <v>0.33879999999999999</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="40">
+      <c r="E12" s="3">
         <v>1.3046</v>
       </c>
-      <c r="F12" s="40">
+      <c r="F12" s="3">
         <v>0.66649999999999998</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="11">
         <v>31.229299999999999</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="2">
         <v>8.8300000000000003E-2</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="2">
         <v>0.06</v>
       </c>
       <c r="J12" s="4">
         <v>0.16120000000000001</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="2">
         <v>4.9299999999999997E-2</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="2">
         <v>0.16120000000000001</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="2">
         <v>5.4199999999999998E-2</v>
       </c>
       <c r="N12" s="4">
         <v>0.16120000000000001</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="2">
         <v>0.16120000000000001</v>
       </c>
-      <c r="P12" s="5">
+      <c r="P12" s="2">
         <v>0.16120000000000001</v>
       </c>
       <c r="Q12" s="4">
         <v>0.16120000000000001</v>
       </c>
-      <c r="R12" s="5">
+      <c r="R12" s="2">
         <v>0.15640000000000001</v>
       </c>
-      <c r="S12" s="54">
+      <c r="S12" s="44">
         <v>1.5639000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="56" t="s">
+    <row r="13" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>0.3</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>0.17960000000000001</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="27">
         <v>1.6019000000000001</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>5.0250000000000004</v>
       </c>
-      <c r="F13" s="9">
-        <v>0</v>
-      </c>
-      <c r="G13" s="35">
+      <c r="F13" s="8">
+        <v>0</v>
+      </c>
+      <c r="G13" s="27">
         <v>-24.595600000000001</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <v>-0.23599999999999999</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <v>0.06</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="6">
         <v>0.13200000000000001</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="7">
         <v>3.2399999999999998E-2</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="7">
         <v>-8.9800000000000005E-2</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M13" s="7">
         <v>8.2699999999999996E-2</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="6">
         <v>0.12039999999999999</v>
       </c>
-      <c r="O13" s="8">
+      <c r="O13" s="7">
         <v>-7.9600000000000004E-2</v>
       </c>
-      <c r="P13" s="8">
+      <c r="P13" s="7">
         <v>-0.68459999999999999</v>
       </c>
-      <c r="Q13" s="7">
+      <c r="Q13" s="6">
         <v>0.12039999999999999</v>
       </c>
-      <c r="R13" s="8">
+      <c r="R13" s="7">
         <v>0.15</v>
       </c>
-      <c r="S13" s="57">
+      <c r="S13" s="47">
         <v>1.4997</v>
       </c>
-      <c r="T13" s="8"/>
-    </row>
-    <row r="15" spans="1:21" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="27" t="s">
+      <c r="T13" s="7"/>
+    </row>
+    <row r="15" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18"/>
+      <c r="C15" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="29" t="str">
+      <c r="D15" s="21"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="22" t="str">
         <f>G1</f>
         <v xml:space="preserve"> Decl</v>
       </c>
-      <c r="H15" s="33" t="str">
+      <c r="H15" s="25" t="str">
         <f>H1</f>
         <v xml:space="preserve"> LO</v>
       </c>
-      <c r="I15" s="31" t="str">
+      <c r="I15" s="9" t="str">
         <f>I1</f>
         <v xml:space="preserve"> MM</v>
       </c>
-      <c r="J15" s="29" t="str">
+      <c r="J15" s="22" t="str">
         <f>J1</f>
         <v xml:space="preserve"> BS_50</v>
       </c>
-      <c r="K15" s="30" t="str">
+      <c r="K15" s="23" t="str">
         <f t="shared" ref="K15:O15" si="0">K1</f>
         <v xml:space="preserve"> BV_50</v>
       </c>
-      <c r="L15" s="31" t="str">
+      <c r="L15" s="9" t="str">
         <f>L1</f>
         <v>β</v>
       </c>
-      <c r="M15" s="30" t="str">
+      <c r="M15" s="23" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> GS</v>
       </c>
-      <c r="N15" s="32" t="str">
+      <c r="N15" s="24" t="str">
         <f>N1</f>
         <v xml:space="preserve"> PR</v>
       </c>
-      <c r="O15" s="31" t="str">
+      <c r="O15" s="9" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> EG</v>
       </c>
-      <c r="P15" s="31" t="str">
+      <c r="P15" s="9" t="str">
         <f>P1</f>
         <v>𝛾</v>
       </c>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="6" t="s">
+      <c r="Q15" s="6"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="17"/>
+      <c r="A16" s="14"/>
+      <c r="B16"/>
       <c r="C16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="21" t="str">
+      <c r="D16" s="4"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="16" t="str">
         <f t="shared" ref="G16:I27" si="1">IF(OR(AND($R2 &gt; 0, G2 &lt; 0), AND($R2 &lt; 0, G2 &gt; 0)), "*", "")</f>
         <v>*</v>
       </c>
-      <c r="H16" s="20" t="str">
+      <c r="H16" s="15" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="I16" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J16" s="21" t="str">
+      <c r="I16" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J16" s="16" t="str">
         <f t="shared" ref="J16:P27" si="2">IF(OR(AND($R2 &gt; 0, J2 &lt; 0), AND($R2 &lt; 0, J2 &gt; 0)), "X", "")</f>
         <v/>
       </c>
-      <c r="K16" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L16" s="20" t="str">
+      <c r="K16" s="15" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L16" s="15" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="M16" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N16" s="21" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O16" s="41" t="str">
+      <c r="M16" s="15" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N16" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O16" s="32" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="P16" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="P16" s="15" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="44" t="str">
+      <c r="G17" s="35" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="H17" s="37" t="str">
+      <c r="H17" s="29" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="I17" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J17" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K17" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L17" s="46" t="str">
+      <c r="I17" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J17" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K17" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L17" s="29" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="M17" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N17" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O17" s="42" t="str">
+      <c r="M17" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N17" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O17" s="33" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="P17" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="P17" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="44" t="str">
+      <c r="G18" s="35" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="H18" s="37" t="str">
+      <c r="H18" s="29" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="I18" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J18" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K18" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L18" s="46" t="str">
+      <c r="I18" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J18" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K18" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L18" s="29" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="M18" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N18" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O18" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P18" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="M18" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N18" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O18" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P18" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="44" t="str">
+      <c r="G19" s="35" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="H19" s="37" t="str">
+      <c r="H19" s="29" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="I19" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J19" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K19" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L19" s="46" t="str">
+      <c r="I19" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J19" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K19" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L19" s="29" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="M19" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N19" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O19" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P19" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="M19" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N19" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O19" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P19" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="44" t="str">
+      <c r="G20" s="35" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="H20" s="37" t="str">
+      <c r="H20" s="29" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="I20" s="37" t="str">
+      <c r="I20" s="29" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="J20" s="36" t="str">
+      <c r="J20" s="28" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="K20" s="37" t="str">
+      <c r="K20" s="29" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="L20" s="46" t="str">
+      <c r="L20" s="29" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="M20" s="37" t="str">
+      <c r="M20" s="29" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="N20" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O20" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P20" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="U20" s="17"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="N20" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O20" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P20" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="44" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H21" s="37" t="str">
+      <c r="G21" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H21" s="29" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="I21" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J21" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K21" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L21" s="46" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M21" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N21" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O21" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P21" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="U21" s="17"/>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="I21" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J21" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K21" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L21" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="M21" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N21" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O21" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P21" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="44" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H22" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I22" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J22" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K22" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L22" s="46" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M22" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N22" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O22" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P22" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="U22" s="17"/>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="G22" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H22" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I22" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J22" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K22" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L22" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="M22" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N22" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O22" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P22" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="44" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H23" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I23" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J23" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K23" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L23" s="46" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M23" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N23" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O23" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P23" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="U23" s="17"/>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="G23" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H23" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I23" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J23" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K23" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L23" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="M23" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N23" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O23" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P23" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G24" s="44" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H24" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I24" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J24" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K24" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L24" s="46" t="str">
+      <c r="G24" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H24" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I24" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J24" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K24" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L24" s="29" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="M24" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N24" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O24" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P24" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="U24" s="17"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="M24" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N24" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O24" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P24" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G25" s="44" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H25" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I25" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J25" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K25" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L25" s="46" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M25" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N25" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O25" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P25" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="U25" s="17"/>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="G25" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H25" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I25" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J25" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K25" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L25" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="M25" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N25" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O25" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P25" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G26" s="44" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H26" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I26" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J26" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K26" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L26" s="46" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M26" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N26" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O26" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P26" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="U26" s="17"/>
-    </row>
-    <row r="27" spans="2:21" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="7"/>
-      <c r="C27" s="34" t="s">
+      <c r="G26" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H26" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I26" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J26" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K26" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L26" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="M26" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N26" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O26" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P26" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="6"/>
+      <c r="C27" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="35"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="45" t="str">
+      <c r="D27" s="27"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="36" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="H27" s="39" t="str">
+      <c r="H27" s="31" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="I27" s="39" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J27" s="38" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K27" s="39" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L27" s="39" t="str">
+      <c r="I27" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J27" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K27" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L27" s="31" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="M27" s="39" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N27" s="65" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O27" s="43" t="str">
+      <c r="M27" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N27" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O27" s="34" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="P27" s="43" t="str">
+      <c r="P27" s="34" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
-      <c r="U27" s="24"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2643,940 +2640,938 @@
     <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" style="3" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.83203125" style="2" customWidth="1"/>
     <col min="10" max="10" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.83203125" style="46" customWidth="1"/>
-    <col min="21" max="21" width="3.83203125" style="5" customWidth="1"/>
-    <col min="22" max="22" width="10.83203125" style="18"/>
+    <col min="18" max="18" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.83203125" style="29" customWidth="1"/>
+    <col min="21" max="21" width="3.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="49" t="s">
+      <c r="B1" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="M1" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="48" t="s">
+      <c r="N1" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="49" t="s">
+      <c r="O1" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="111" t="s">
+      <c r="P1" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="Q1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="49" t="s">
+      <c r="R1" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="52" t="s">
+      <c r="S1" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="68" t="s">
+      <c r="T1" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="U1" s="10"/>
-      <c r="V1" s="6" t="s">
+      <c r="U1" s="9"/>
+      <c r="V1" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="104">
+      <c r="B2" s="94">
         <v>0.6</v>
       </c>
-      <c r="C2" s="60">
+      <c r="C2" s="95">
         <v>0.60029999999999994</v>
       </c>
-      <c r="D2" s="101">
+      <c r="D2" s="96">
         <v>1.0033000000000001</v>
       </c>
-      <c r="E2" s="62">
+      <c r="E2" s="97">
         <v>0.84309999999999996</v>
       </c>
-      <c r="F2" s="62">
+      <c r="F2" s="97">
         <v>0.98609999999999998</v>
       </c>
-      <c r="G2" s="61">
+      <c r="G2" s="98">
         <v>4.9264000000000001</v>
       </c>
-      <c r="H2" s="60">
+      <c r="H2" s="95">
         <v>0.1171</v>
       </c>
-      <c r="I2" s="60">
-        <v>0</v>
-      </c>
-      <c r="J2" s="59">
-        <v>0</v>
-      </c>
-      <c r="K2" s="60">
-        <v>0</v>
-      </c>
-      <c r="L2" s="60">
+      <c r="I2" s="95">
+        <v>0</v>
+      </c>
+      <c r="J2" s="94">
+        <v>0</v>
+      </c>
+      <c r="K2" s="95">
+        <v>0</v>
+      </c>
+      <c r="L2" s="95">
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="M2" s="60">
+      <c r="M2" s="95">
         <v>-3.6299999999999999E-2</v>
       </c>
-      <c r="N2" s="59">
+      <c r="N2" s="94">
         <v>-2.9999999999999997E-4</v>
       </c>
-      <c r="O2" s="74">
+      <c r="O2" s="95">
         <v>9.9699999999999997E-2</v>
       </c>
-      <c r="P2" s="112">
+      <c r="P2" s="99">
         <v>-1.6E-2</v>
       </c>
-      <c r="Q2" s="59">
+      <c r="Q2" s="49">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="R2" s="60">
+      <c r="R2" s="50">
         <v>-6.7999999999999996E-3</v>
       </c>
-      <c r="S2" s="63">
+      <c r="S2" s="53">
         <v>-0.15540000000000001</v>
       </c>
-      <c r="T2" s="69" t="s">
+      <c r="T2" s="56" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="105">
+      <c r="B3" s="101">
         <v>0.6</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="102">
         <v>0.69199999999999995</v>
       </c>
-      <c r="D3" s="102">
+      <c r="D3" s="103">
         <v>1.92</v>
       </c>
-      <c r="E3" s="40">
+      <c r="E3" s="104">
         <v>1.6133999999999999</v>
       </c>
-      <c r="F3" s="40">
+      <c r="F3" s="104">
         <v>0.41980000000000001</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="105">
         <v>1.2159</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="102">
         <v>0.1028</v>
       </c>
-      <c r="I3" s="5">
-        <v>0</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0</v>
-      </c>
-      <c r="K3" s="5">
-        <v>0</v>
-      </c>
-      <c r="L3" s="5">
+      <c r="I3" s="102">
+        <v>0</v>
+      </c>
+      <c r="J3" s="101">
+        <v>0</v>
+      </c>
+      <c r="K3" s="102">
+        <v>0</v>
+      </c>
+      <c r="L3" s="102">
         <v>4.7300000000000002E-2</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="102">
         <v>-2.64E-2</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="101">
         <v>-9.1999999999999998E-2</v>
       </c>
-      <c r="O3" s="75">
+      <c r="O3" s="102">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="P3" s="113">
+      <c r="P3" s="106">
         <v>-3.0700000000000002E-2</v>
       </c>
       <c r="Q3" s="4">
         <v>-9.1999999999999998E-2</v>
       </c>
-      <c r="R3" s="5">
+      <c r="R3" s="2">
         <v>-9.9900000000000003E-2</v>
       </c>
-      <c r="S3" s="54">
+      <c r="S3" s="44">
         <v>-2.4965000000000002</v>
       </c>
-      <c r="T3" s="70" t="s">
+      <c r="T3" s="57" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="105">
+      <c r="B4" s="101">
         <v>0.6</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="102">
         <v>0.79769999999999996</v>
       </c>
-      <c r="D4" s="72">
+      <c r="D4" s="103">
         <v>2.9767000000000001</v>
       </c>
-      <c r="E4" s="40">
+      <c r="E4" s="104">
         <v>2.4315000000000002</v>
       </c>
-      <c r="F4" s="40">
+      <c r="F4" s="104">
         <v>0.21129999999999999</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="105">
         <v>5.944</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="102">
         <v>0.109</v>
       </c>
-      <c r="I4" s="5">
-        <v>0</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0</v>
-      </c>
-      <c r="L4" s="5">
+      <c r="I4" s="102">
+        <v>0</v>
+      </c>
+      <c r="J4" s="101">
+        <v>0</v>
+      </c>
+      <c r="K4" s="102">
+        <v>0</v>
+      </c>
+      <c r="L4" s="102">
         <v>5.1499999999999997E-2</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="102">
         <v>-1.7299999999999999E-2</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="101">
         <v>-0.19769999999999999</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="102">
         <v>-9.7699999999999995E-2</v>
       </c>
-      <c r="P4" s="113">
+      <c r="P4" s="106">
         <v>-5.45E-2</v>
       </c>
       <c r="Q4" s="4">
         <v>-0.19769999999999999</v>
       </c>
-      <c r="R4" s="5">
+      <c r="R4" s="2">
         <v>-0.2041</v>
       </c>
-      <c r="S4" s="54">
+      <c r="S4" s="44">
         <v>-5.1029999999999998</v>
       </c>
-      <c r="T4" s="70" t="s">
+      <c r="T4" s="57" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="105">
+      <c r="B5" s="101">
         <v>0.64</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="102">
         <v>0.98380000000000001</v>
       </c>
-      <c r="D5" s="72">
+      <c r="D5" s="103">
         <v>3.456</v>
       </c>
-      <c r="E5" s="40">
+      <c r="E5" s="104">
         <v>0.74709999999999999</v>
       </c>
-      <c r="F5" s="40">
+      <c r="F5" s="104">
         <v>1.1385000000000001</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="55" t="s">
+      <c r="H5" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="4">
-        <v>0</v>
-      </c>
-      <c r="K5" s="5">
-        <v>0</v>
-      </c>
-      <c r="L5" s="5">
+      <c r="I5" s="102">
+        <v>0</v>
+      </c>
+      <c r="J5" s="101">
+        <v>0</v>
+      </c>
+      <c r="K5" s="102">
+        <v>0</v>
+      </c>
+      <c r="L5" s="102">
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="102">
         <v>-8.0000000000000002E-3</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="101">
         <v>-0.34379999999999999</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="102">
         <v>-0.20380000000000001</v>
       </c>
-      <c r="P5" s="113">
+      <c r="P5" s="106">
         <v>-0.37919999999999998</v>
       </c>
       <c r="Q5" s="4">
         <v>-0.38379999999999997</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5" s="2">
         <v>-0.35410000000000003</v>
       </c>
-      <c r="S5" s="54">
+      <c r="S5" s="44">
         <v>-3.5405000000000002</v>
       </c>
-      <c r="T5" s="70" t="s">
+      <c r="T5" s="57" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="101">
         <v>0.52</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="102">
         <v>0.66649999999999998</v>
       </c>
-      <c r="D6" s="72">
+      <c r="D6" s="103">
         <v>8.3239000000000001</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="104">
         <v>8.0289000000000001</v>
       </c>
-      <c r="F6" s="40">
+      <c r="F6" s="104">
         <v>2.46E-2</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="102">
         <v>2.58E-2</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="102">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="101">
         <v>1.5E-3</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="102">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="102">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="102">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="101">
         <v>-0.14649999999999999</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="102">
         <v>-0.1265</v>
       </c>
-      <c r="P6" s="113">
+      <c r="P6" s="106">
         <v>-5.8999999999999999E-3</v>
       </c>
       <c r="Q6" s="4">
         <v>-0.16650000000000001</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R6" s="2">
         <v>-0.13150000000000001</v>
       </c>
-      <c r="S6" s="54">
+      <c r="S6" s="44">
         <v>-1.5783</v>
       </c>
-      <c r="T6" s="70" t="s">
+      <c r="T6" s="57" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="101">
         <v>0.51</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="102">
         <v>0.56569999999999998</v>
       </c>
-      <c r="D7" s="72">
+      <c r="D7" s="103">
         <v>6.5736999999999997</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="104">
         <v>4.9969999999999999</v>
       </c>
-      <c r="F7" s="40">
+      <c r="F7" s="104">
         <v>0.10009999999999999</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="105">
         <v>-0.7359</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="102">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="102">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="101">
         <v>-1.49E-2</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="102">
         <v>-2.8E-3</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="102">
         <v>-1.34E-2</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="102">
         <v>-3.5999999999999999E-3</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="101">
         <v>-5.57E-2</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="102">
         <v>-4.5699999999999998E-2</v>
       </c>
-      <c r="P7" s="113">
+      <c r="P7" s="106">
         <v>-1.5800000000000002E-2</v>
       </c>
       <c r="Q7" s="4">
         <v>-6.5699999999999995E-2</v>
       </c>
-      <c r="R7" s="5">
+      <c r="R7" s="2">
         <v>-0.05</v>
       </c>
-      <c r="S7" s="54">
+      <c r="S7" s="44">
         <v>-0.4995</v>
       </c>
-      <c r="T7" s="70" t="s">
+      <c r="T7" s="57" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="101">
         <v>0.52300000000000002</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="102">
         <v>0.59930000000000005</v>
       </c>
-      <c r="D8" s="72">
+      <c r="D8" s="103">
         <v>4.3182999999999998</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="104">
         <v>5.4100000000000002E-2</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="104">
         <v>18.401199999999999</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="105">
         <v>-15.289400000000001</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="102">
         <v>-2.9399999999999999E-2</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="102">
         <v>-9.1999999999999998E-2</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="101">
         <v>-9.6100000000000005E-2</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="102">
         <v>-6.7000000000000004E-2</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="102">
         <v>-9.1800000000000007E-2</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="102">
         <v>-4.6100000000000002E-2</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8" s="101">
         <v>-7.6300000000000007E-2</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="102">
         <v>-5.33E-2</v>
       </c>
-      <c r="P8" s="113">
+      <c r="P8" s="106">
         <v>-9.8100000000000007E-2</v>
       </c>
       <c r="Q8" s="4">
         <v>-9.9299999999999999E-2</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="2">
         <v>-9.8500000000000004E-2</v>
       </c>
-      <c r="S8" s="54">
+      <c r="S8" s="44">
         <v>-0.98529999999999995</v>
       </c>
-      <c r="T8" s="70" t="s">
+      <c r="T8" s="57" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="101">
         <v>0.52300000000000002</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="102">
         <v>0.6</v>
       </c>
-      <c r="D9" s="72">
+      <c r="D9" s="103">
         <v>4.3478000000000003</v>
       </c>
-      <c r="E9" s="40">
-        <v>0</v>
-      </c>
-      <c r="F9" s="66" t="s">
+      <c r="E9" s="104">
+        <v>0</v>
+      </c>
+      <c r="F9" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="105">
         <v>-18.093499999999999</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="102">
         <v>-0.08</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="102">
         <v>-0.192</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="101">
         <v>-0.1</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="102">
         <v>-0.12609999999999999</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="102">
         <v>-0.1</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="102">
         <v>-7.9699999999999993E-2</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="101">
         <v>-7.6999999999999999E-2</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O9" s="102">
         <v>-5.3999999999999999E-2</v>
       </c>
-      <c r="P9" s="113">
+      <c r="P9" s="106">
         <v>-0.1</v>
       </c>
       <c r="Q9" s="4">
         <v>-0.1</v>
       </c>
-      <c r="R9" s="5">
+      <c r="R9" s="2">
         <v>-0.1</v>
       </c>
-      <c r="S9" s="54">
+      <c r="S9" s="44">
         <v>-1</v>
       </c>
-      <c r="T9" s="70" t="s">
+      <c r="T9" s="57" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="101">
         <v>0.56999999999999995</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="102">
         <v>0.73980000000000001</v>
       </c>
-      <c r="D10" s="72">
+      <c r="D10" s="103">
         <v>3.4262000000000001</v>
       </c>
-      <c r="E10" s="40">
+      <c r="E10" s="104">
         <v>1.9415</v>
       </c>
-      <c r="F10" s="40">
+      <c r="F10" s="104">
         <v>0.31509999999999999</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="105">
         <v>-29.989699999999999</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="102">
         <v>-1.6E-2</v>
       </c>
-      <c r="I10" s="5">
-        <v>0</v>
-      </c>
-      <c r="J10" s="4">
-        <v>0</v>
-      </c>
-      <c r="K10" s="5">
-        <v>0</v>
-      </c>
-      <c r="L10" s="5">
+      <c r="I10" s="102">
+        <v>0</v>
+      </c>
+      <c r="J10" s="101">
+        <v>0</v>
+      </c>
+      <c r="K10" s="102">
+        <v>0</v>
+      </c>
+      <c r="L10" s="102">
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="102">
         <v>-1.3899999999999999E-2</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10" s="101">
         <v>-0.16980000000000001</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="102">
         <v>-9.98E-2</v>
       </c>
-      <c r="P10" s="113">
+      <c r="P10" s="106">
         <v>-0.10390000000000001</v>
       </c>
       <c r="Q10" s="4">
         <v>-0.13980000000000001</v>
       </c>
-      <c r="R10" s="5">
+      <c r="R10" s="2">
         <v>-0.15509999999999999</v>
       </c>
-      <c r="S10" s="54">
+      <c r="S10" s="44">
         <v>-1.5513999999999999</v>
       </c>
-      <c r="T10" s="70" t="s">
+      <c r="T10" s="57" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="101">
         <v>0.443</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="102">
         <v>0.55600000000000005</v>
       </c>
-      <c r="D11" s="72">
+      <c r="D11" s="103">
         <v>-0.98219999999999996</v>
       </c>
-      <c r="E11" s="40">
+      <c r="E11" s="104">
         <v>1.6238999999999999</v>
       </c>
-      <c r="F11" s="40">
+      <c r="F11" s="104">
         <v>0.4158</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="105">
         <v>-29.011500000000002</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="102">
         <v>-0.15359999999999999</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="102">
         <v>-9.1999999999999998E-2</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="101">
         <v>-9.4899999999999998E-2</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="102">
         <v>-0.08</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="102">
         <v>-7.8299999999999995E-2</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="102">
         <v>-3.3599999999999998E-2</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11" s="101">
         <v>-0.113</v>
       </c>
-      <c r="O11" s="5">
+      <c r="O11" s="102">
         <v>-0.17</v>
       </c>
-      <c r="P11" s="113">
+      <c r="P11" s="106">
         <v>-0.14849999999999999</v>
       </c>
       <c r="Q11" s="4">
         <v>-0.156</v>
       </c>
-      <c r="R11" s="5">
+      <c r="R11" s="2">
         <v>-0.1118</v>
       </c>
-      <c r="S11" s="54">
+      <c r="S11" s="44">
         <v>-1.1185</v>
       </c>
-      <c r="T11" s="70" t="s">
+      <c r="T11" s="57" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="101">
         <v>0.5</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="102">
         <v>0.33879999999999999</v>
       </c>
-      <c r="D12" s="73" t="s">
+      <c r="D12" s="110" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="40">
+      <c r="E12" s="104">
         <v>1.3046</v>
       </c>
-      <c r="F12" s="40">
+      <c r="F12" s="104">
         <v>0.66649999999999998</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="105">
         <v>31.229299999999999</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="102">
         <v>8.8300000000000003E-2</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="102">
         <v>0.06</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="101">
         <v>0.16120000000000001</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="102">
         <v>4.9299999999999997E-2</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="102">
         <v>0.16120000000000001</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="102">
         <v>5.4199999999999998E-2</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12" s="101">
         <v>0.16120000000000001</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="102">
         <v>0.16120000000000001</v>
       </c>
-      <c r="P12" s="113">
+      <c r="P12" s="106">
         <v>0.16120000000000001</v>
       </c>
       <c r="Q12" s="4">
         <v>0.16120000000000001</v>
       </c>
-      <c r="R12" s="5">
+      <c r="R12" s="2">
         <v>0.15640000000000001</v>
       </c>
-      <c r="S12" s="54">
+      <c r="S12" s="44">
         <v>1.5639000000000001</v>
       </c>
-      <c r="T12" s="70" t="s">
+      <c r="T12" s="57" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="56" t="s">
+    <row r="13" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="112">
         <v>0.3</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="113">
         <v>0.17960000000000001</v>
       </c>
-      <c r="D13" s="103">
+      <c r="D13" s="114">
         <v>1.6019000000000001</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="115">
         <v>5.0250000000000004</v>
       </c>
-      <c r="F13" s="9">
-        <v>0</v>
-      </c>
-      <c r="G13" s="35">
+      <c r="F13" s="115">
+        <v>0</v>
+      </c>
+      <c r="G13" s="116">
         <v>-24.595600000000001</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="113">
         <v>-0.23599999999999999</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="113">
         <v>0.06</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="112">
         <v>0.13200000000000001</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="113">
         <v>3.2399999999999998E-2</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="113">
         <v>-8.9800000000000005E-2</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M13" s="113">
         <v>8.2699999999999996E-2</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="112">
         <v>0.12039999999999999</v>
       </c>
-      <c r="O13" s="76">
+      <c r="O13" s="113">
         <v>-7.9600000000000004E-2</v>
       </c>
-      <c r="P13" s="114">
+      <c r="P13" s="117">
         <v>-0.68459999999999999</v>
       </c>
-      <c r="Q13" s="7">
+      <c r="Q13" s="6">
         <v>0.12039999999999999</v>
       </c>
-      <c r="R13" s="8">
+      <c r="R13" s="7">
         <v>0.15</v>
       </c>
-      <c r="S13" s="57">
+      <c r="S13" s="47">
         <v>1.4997</v>
       </c>
-      <c r="T13" s="71" t="s">
+      <c r="T13" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="U13" s="8"/>
-    </row>
-    <row r="15" spans="1:22" s="22" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="27" t="s">
+      <c r="U13" s="7"/>
+    </row>
+    <row r="15" spans="1:22" s="17" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="C15" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="91" t="str">
+      <c r="D15" s="21"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="72" t="str">
         <f>G1</f>
         <v xml:space="preserve"> Decl</v>
       </c>
-      <c r="H15" s="92" t="str">
+      <c r="H15" s="73" t="str">
         <f>H1</f>
         <v xml:space="preserve"> LO</v>
       </c>
-      <c r="I15" s="93" t="str">
+      <c r="I15" s="74" t="str">
         <f>I1</f>
         <v xml:space="preserve"> MM</v>
       </c>
-      <c r="J15" s="94" t="str">
+      <c r="J15" s="75" t="str">
         <f>J1</f>
         <v xml:space="preserve"> BS_50</v>
       </c>
-      <c r="K15" s="95" t="str">
+      <c r="K15" s="76" t="str">
         <f t="shared" ref="K15:O15" si="0">K1</f>
         <v xml:space="preserve"> BV_50</v>
       </c>
-      <c r="L15" s="96" t="str">
+      <c r="L15" s="77" t="str">
         <f>L1</f>
         <v>β</v>
       </c>
-      <c r="M15" s="95" t="str">
+      <c r="M15" s="76" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> GS</v>
       </c>
-      <c r="N15" s="32" t="str">
+      <c r="N15" s="24" t="str">
         <f>N1</f>
         <v xml:space="preserve"> PR</v>
       </c>
-      <c r="O15" s="100" t="str">
+      <c r="O15" s="81" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> EG</v>
       </c>
-      <c r="P15" s="31" t="str">
+      <c r="P15" s="9" t="str">
         <f>P1</f>
         <v>𝛾</v>
       </c>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="39"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="6" t="s">
+      <c r="Q15" s="6"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="31"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="17"/>
+      <c r="A16" s="14"/>
+      <c r="B16"/>
       <c r="C16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="77" t="str">
+      <c r="D16" s="4"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="59" t="str">
         <f t="shared" ref="G16:I27" si="1">IF(OR(AND($R2 &gt; 0, G2 &lt; 0), AND($R2 &lt; 0, G2 &gt; 0)), "*", "")</f>
         <v>*</v>
       </c>
-      <c r="H16" s="78" t="str">
+      <c r="H16" s="60" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="I16" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J16" s="106" t="s">
+      <c r="I16" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J16" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="20" t="str">
+      <c r="K16" s="15" t="str">
         <f t="shared" ref="J16:P27" si="2">IF(OR(AND($R2 &gt; 0, K2 &lt; 0), AND($R2 &lt; 0, K2 &gt; 0)), "X", "")</f>
         <v/>
       </c>
-      <c r="L16" s="97" t="str">
+      <c r="L16" s="78" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="M16" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N16" s="21" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O16" s="109" t="str">
+      <c r="M16" s="15" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N16" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O16" s="85" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="P16" s="20" t="str">
+      <c r="P16" s="15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3585,42 +3580,42 @@
       <c r="C17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="83" t="str">
+      <c r="G17" s="35" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="H17" s="67" t="str">
+      <c r="H17" s="29" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="I17" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J17" s="107" t="s">
+      <c r="I17" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J17" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="K17" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L17" s="98" t="str">
+      <c r="K17" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L17" s="79" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="M17" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N17" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O17" s="110" t="str">
+      <c r="M17" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N17" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O17" s="86" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="P17" s="67" t="str">
+      <c r="P17" s="29" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3629,87 +3624,86 @@
       <c r="C18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="44" t="str">
+      <c r="G18" s="35" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="H18" s="37" t="str">
+      <c r="H18" s="29" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="I18" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J18" s="107" t="s">
+      <c r="I18" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J18" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="K18" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L18" s="98" t="str">
+      <c r="K18" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L18" s="79" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="M18" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N18" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O18" s="67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P18" s="67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="V18" s="17"/>
+      <c r="M18" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N18" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O18" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P18" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="81" t="str">
+      <c r="G19" s="63" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="H19" s="82" t="str">
+      <c r="H19" s="64" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="I19" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J19" s="107" t="s">
+      <c r="I19" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J19" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="K19" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L19" s="98" t="str">
+      <c r="K19" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L19" s="79" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="M19" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N19" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O19" s="67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P19" s="67" t="str">
+      <c r="M19" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N19" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O19" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P19" s="29" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3718,46 +3712,46 @@
       <c r="C20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="81" t="str">
+      <c r="G20" s="63" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="H20" s="37" t="str">
+      <c r="H20" s="29" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="I20" s="37" t="str">
+      <c r="I20" s="29" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="J20" s="107" t="s">
+      <c r="J20" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="K20" s="37" t="str">
+      <c r="K20" s="29" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="L20" s="98" t="str">
+      <c r="L20" s="79" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="M20" s="37" t="str">
+      <c r="M20" s="29" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="N20" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O20" s="67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P20" s="67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="V20" s="17" t="s">
+      <c r="N20" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O20" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P20" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="V20" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3765,376 +3759,369 @@
       <c r="C21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="44" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H21" s="37" t="str">
+      <c r="G21" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H21" s="29" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="I21" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J21" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K21" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L21" s="46" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M21" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N21" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O21" s="67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P21" s="67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="V21" s="17"/>
+      <c r="I21" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J21" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K21" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L21" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="M21" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N21" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O21" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P21" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="44" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H22" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I22" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J22" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K22" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L22" s="46" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M22" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N22" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O22" s="67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P22" s="67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="V22" s="17"/>
+      <c r="G22" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H22" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I22" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J22" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K22" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L22" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="M22" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N22" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O22" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P22" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="44" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H23" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I23" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J23" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K23" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L23" s="46" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M23" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N23" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O23" s="67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P23" s="67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="V23" s="17"/>
+      <c r="G23" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H23" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I23" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J23" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K23" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L23" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="M23" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N23" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O23" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P23" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G24" s="44" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H24" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I24" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J24" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K24" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L24" s="98" t="str">
+      <c r="G24" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H24" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I24" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J24" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K24" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L24" s="79" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="M24" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N24" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O24" s="67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P24" s="67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="V24" s="17"/>
+      <c r="M24" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N24" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O24" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P24" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G25" s="44" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H25" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I25" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J25" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K25" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L25" s="46" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M25" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N25" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O25" s="67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P25" s="67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="V25" s="17"/>
+      <c r="G25" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H25" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I25" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J25" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K25" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L25" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="M25" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N25" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O25" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P25" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="26" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G26" s="44" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H26" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I26" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J26" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K26" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L26" s="46" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M26" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N26" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O26" s="67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="P26" s="67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="V26" s="17"/>
-    </row>
-    <row r="27" spans="2:22" s="22" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="34" t="s">
+      <c r="G26" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H26" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I26" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J26" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K26" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L26" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="M26" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N26" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O26" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P26" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="2:22" s="17" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
+      <c r="C27" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="35"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="79" t="str">
+      <c r="D27" s="27"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="61" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="H27" s="80" t="str">
+      <c r="H27" s="62" t="str">
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="I27" s="39" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J27" s="38" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="K27" s="39" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L27" s="99" t="str">
+      <c r="I27" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J27" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K27" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L27" s="80" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="M27" s="39" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N27" s="65" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O27" s="110" t="str">
+      <c r="M27" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N27" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O27" s="86" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="P27" s="110" t="str">
+      <c r="P27" s="86" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="39"/>
-      <c r="U27" s="8"/>
-      <c r="V27" s="24"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="31"/>
+      <c r="U27" s="7"/>
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="D31" s="84"/>
-      <c r="E31" s="85" t="s">
+      <c r="D31" s="65"/>
+      <c r="E31" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="86"/>
-      <c r="G31" s="87" t="s">
+      <c r="F31" s="67"/>
+      <c r="G31" s="68" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="D32" s="88"/>
-      <c r="E32" s="85" t="s">
+      <c r="D32" s="69"/>
+      <c r="E32" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="F32" s="86"/>
-      <c r="G32" s="87" t="s">
+      <c r="F32" s="67"/>
+      <c r="G32" s="68" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D33" s="89"/>
-      <c r="E33" s="85" t="s">
+      <c r="D33" s="70"/>
+      <c r="E33" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="F33" s="86"/>
-      <c r="G33" s="87" t="s">
+      <c r="F33" s="67"/>
+      <c r="G33" s="68" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D34" s="90"/>
-      <c r="E34" s="85" t="s">
+      <c r="D34" s="71"/>
+      <c r="E34" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="F34" s="86"/>
-      <c r="G34" s="87" t="s">
+      <c r="F34" s="67"/>
+      <c r="G34" s="68" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="35" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D35" s="108"/>
-      <c r="G35" s="12" t="s">
+      <c r="D35" s="84"/>
+      <c r="G35" s="11" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>